<commit_message>
update the RAS file with BioRECIPE format
</commit_message>
<xml_diff>
--- a/examples/models/RAS_biorecipes_scenario_detailed.xlsx
+++ b/examples/models/RAS_biorecipes_scenario_detailed.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaoxiangzhou/Downloads/BioRECIPES/examples/models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasmine/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDA0F19-FDE7-6646-B36F-30F27D6FAE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB821376-21F4-9243-AD2E-2B824CA702D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8160" yWindow="4120" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AO$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$AP$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
   <si>
     <t>Update Group</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>ERK</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -316,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -361,6 +364,17 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,776 +679,855 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ63"/>
+  <dimension ref="A1:AR63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.5" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="22.5" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="46" customWidth="1"/>
-    <col min="7" max="8" width="22.33203125" customWidth="1"/>
-    <col min="10" max="12" width="22.33203125" customWidth="1"/>
-    <col min="13" max="13" width="24.83203125" customWidth="1"/>
-    <col min="14" max="14" width="28.33203125" customWidth="1"/>
-    <col min="15" max="15" width="26.33203125" customWidth="1"/>
-    <col min="16" max="16" width="17" customWidth="1"/>
-    <col min="17" max="17" width="24.83203125" customWidth="1"/>
-    <col min="18" max="18" width="31.1640625" customWidth="1"/>
-    <col min="19" max="19" width="22.33203125" customWidth="1"/>
-    <col min="20" max="20" width="23.33203125" customWidth="1"/>
-    <col min="21" max="22" width="17.1640625" customWidth="1"/>
-    <col min="23" max="24" width="23.33203125" customWidth="1"/>
-    <col min="25" max="25" width="34.83203125" customWidth="1"/>
-    <col min="26" max="26" width="32" customWidth="1"/>
-    <col min="27" max="27" width="12.83203125" customWidth="1"/>
-    <col min="28" max="28" width="20.83203125" customWidth="1"/>
-    <col min="29" max="29" width="14.5" customWidth="1"/>
-    <col min="30" max="32" width="24.1640625" customWidth="1"/>
-    <col min="36" max="36" width="21.1640625" customWidth="1"/>
-    <col min="39" max="39" width="23.6640625" customWidth="1"/>
-    <col min="40" max="40" width="23.1640625" customWidth="1"/>
-    <col min="41" max="41" width="27.5" customWidth="1"/>
-    <col min="42" max="42" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="48.6640625" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="7" max="7" width="46" customWidth="1"/>
+    <col min="8" max="9" width="22.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
+    <col min="11" max="13" width="22.33203125" customWidth="1"/>
+    <col min="14" max="14" width="24.83203125" customWidth="1"/>
+    <col min="15" max="15" width="28.33203125" customWidth="1"/>
+    <col min="16" max="16" width="26.33203125" customWidth="1"/>
+    <col min="17" max="17" width="17" customWidth="1"/>
+    <col min="18" max="18" width="24.83203125" customWidth="1"/>
+    <col min="19" max="19" width="40.33203125" customWidth="1"/>
+    <col min="20" max="20" width="22.33203125" customWidth="1"/>
+    <col min="21" max="21" width="23.33203125" customWidth="1"/>
+    <col min="22" max="23" width="17.1640625" customWidth="1"/>
+    <col min="24" max="25" width="23.33203125" customWidth="1"/>
+    <col min="26" max="26" width="34.83203125" customWidth="1"/>
+    <col min="27" max="27" width="32" customWidth="1"/>
+    <col min="28" max="28" width="12.83203125" customWidth="1"/>
+    <col min="29" max="29" width="20.83203125" customWidth="1"/>
+    <col min="30" max="30" width="14.5" customWidth="1"/>
+    <col min="31" max="33" width="24.1640625" customWidth="1"/>
+    <col min="36" max="36" width="26.83203125" customWidth="1"/>
+    <col min="37" max="37" width="21.1640625" customWidth="1"/>
+    <col min="40" max="40" width="23.6640625" customWidth="1"/>
+    <col min="41" max="41" width="23.1640625" customWidth="1"/>
+    <col min="42" max="42" width="27.5" customWidth="1"/>
+    <col min="43" max="43" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="AN1" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="AO1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP1" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:41" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="12" t="s">
+      <c r="D2" s="7"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="AC2" s="15" t="s">
+      <c r="AD2" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AD2">
-        <v>1</v>
-      </c>
       <c r="AE2">
         <v>1</v>
       </c>
-      <c r="AJ2">
+      <c r="AF2">
+        <v>1</v>
+      </c>
+      <c r="AK2">
         <v>50</v>
       </c>
-      <c r="AK2" s="16" t="s">
+      <c r="AL2" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="AL2" s="14"/>
-      <c r="AO2" s="2"/>
-    </row>
-    <row r="3" spans="1:41" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="AM2" s="14"/>
+      <c r="AP2" s="2"/>
+    </row>
+    <row r="3" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="12" t="s">
+      <c r="D3" s="7"/>
+      <c r="Z3" s="12"/>
+      <c r="AA3" s="17"/>
+      <c r="AB3" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="AC3" s="15" t="s">
+      <c r="AD3" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AD3">
-        <v>1</v>
-      </c>
       <c r="AE3">
         <v>1</v>
       </c>
-      <c r="AJ3">
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AK3">
         <v>50</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
         <v>41</v>
       </c>
-      <c r="AO3" s="2"/>
-    </row>
-    <row r="4" spans="1:41" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="AP3" s="2"/>
+    </row>
+    <row r="4" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="Y4" s="12" t="s">
+      <c r="D4" s="7"/>
+      <c r="Z4" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="Z4" s="17" t="s">
+      <c r="AA4" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AA4" s="12" t="s">
+      <c r="AB4" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AC4" s="15" t="s">
+      <c r="AD4" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>0</v>
       </c>
-      <c r="AE4">
-        <v>1</v>
-      </c>
-      <c r="AJ4">
+      <c r="AF4">
+        <v>1</v>
+      </c>
+      <c r="AK4">
         <v>50</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
         <v>42</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AM4" t="s">
         <v>43</v>
       </c>
-      <c r="AO4" s="2"/>
-    </row>
-    <row r="5" spans="1:41" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="AP4" s="2"/>
+    </row>
+    <row r="5" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="Y5" s="12" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="Z5" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AA5" s="12" t="s">
+      <c r="AB5" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="AC5" s="15" t="s">
+      <c r="AD5" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AD5">
+      <c r="AE5">
         <v>0</v>
       </c>
-      <c r="AE5">
-        <v>1</v>
-      </c>
-      <c r="AJ5">
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AK5">
         <v>50</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AL5" t="s">
         <v>41</v>
       </c>
-      <c r="AO5" s="2"/>
-    </row>
-    <row r="6" spans="1:41" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="AP5" s="2"/>
+    </row>
+    <row r="6" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="Y6" s="12" t="s">
+      <c r="D6" s="7"/>
+      <c r="Z6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="12" t="s">
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="AC6" s="15" t="s">
+      <c r="AD6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>0</v>
       </c>
-      <c r="AE6">
-        <v>1</v>
-      </c>
-      <c r="AJ6">
+      <c r="AF6">
+        <v>1</v>
+      </c>
+      <c r="AK6">
         <v>50</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" t="s">
         <v>41</v>
       </c>
-      <c r="AO6" s="2"/>
-    </row>
-    <row r="7" spans="1:41" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="AP6" s="2"/>
+    </row>
+    <row r="7" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="Y7" s="12"/>
+      <c r="D7" s="7"/>
       <c r="Z7" s="12"/>
-      <c r="AA7" s="12" t="s">
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="AC7" s="15" t="s">
+      <c r="AD7" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AD7">
-        <v>1</v>
-      </c>
       <c r="AE7">
         <v>1</v>
       </c>
-      <c r="AJ7">
+      <c r="AF7">
+        <v>1</v>
+      </c>
+      <c r="AK7">
         <v>50</v>
       </c>
-      <c r="AK7" t="s">
+      <c r="AL7" t="s">
         <v>41</v>
       </c>
-      <c r="AO7" s="2"/>
-    </row>
-    <row r="8" spans="1:41" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="AP7" s="2"/>
+    </row>
+    <row r="8" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="Y8" s="12" t="s">
+      <c r="D8" s="7"/>
+      <c r="Z8" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="Z8" s="12" t="s">
+      <c r="AA8" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="AA8" s="12" t="s">
+      <c r="AB8" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="AC8" s="15" t="s">
+      <c r="AD8" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AD8">
+      <c r="AE8">
         <v>0</v>
       </c>
-      <c r="AE8">
-        <v>1</v>
-      </c>
-      <c r="AJ8">
+      <c r="AF8">
+        <v>1</v>
+      </c>
+      <c r="AK8">
         <v>50</v>
       </c>
-      <c r="AK8" t="s">
+      <c r="AL8" t="s">
         <v>42</v>
       </c>
-      <c r="AO8" s="2"/>
-    </row>
-    <row r="9" spans="1:41" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+      <c r="AP8" s="2"/>
+    </row>
+    <row r="9" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="Y9" s="12"/>
+      <c r="D9" s="7"/>
       <c r="Z9" s="12"/>
-      <c r="AA9" s="12" t="s">
+      <c r="AA9" s="12"/>
+      <c r="AB9" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="AC9" s="15" t="s">
+      <c r="AD9" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AD9">
-        <v>1</v>
-      </c>
       <c r="AE9">
         <v>1</v>
       </c>
-      <c r="AJ9">
+      <c r="AF9">
+        <v>1</v>
+      </c>
+      <c r="AK9">
         <v>50</v>
       </c>
-      <c r="AK9" t="s">
+      <c r="AL9" t="s">
         <v>41</v>
       </c>
-      <c r="AL9" t="s">
+      <c r="AM9" t="s">
         <v>43</v>
       </c>
-      <c r="AO9" s="2"/>
-    </row>
-    <row r="10" spans="1:41" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="AP9" s="2"/>
+    </row>
+    <row r="10" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="Y10" s="12" t="s">
+      <c r="D10" s="7"/>
+      <c r="Z10" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="Z10" s="12"/>
-      <c r="AA10" s="12" t="s">
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="AC10" s="15" t="s">
+      <c r="AD10" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AD10">
+      <c r="AE10">
         <v>0</v>
       </c>
-      <c r="AE10">
-        <v>1</v>
-      </c>
-      <c r="AJ10">
+      <c r="AF10">
+        <v>1</v>
+      </c>
+      <c r="AK10">
         <v>50</v>
       </c>
-      <c r="AK10" t="s">
+      <c r="AL10" t="s">
         <v>41</v>
       </c>
-      <c r="AO10" s="2"/>
-    </row>
-    <row r="11" spans="1:41" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+      <c r="AP10" s="2"/>
+    </row>
+    <row r="11" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="Y11" s="12"/>
+      <c r="D11" s="7"/>
       <c r="Z11" s="12"/>
-      <c r="AA11" s="12" t="s">
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="AC11" s="15" t="s">
+      <c r="AD11" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AD11">
-        <v>1</v>
-      </c>
       <c r="AE11">
         <v>1</v>
       </c>
-      <c r="AJ11">
+      <c r="AF11">
+        <v>1</v>
+      </c>
+      <c r="AK11">
         <v>50</v>
       </c>
-      <c r="AK11" t="s">
+      <c r="AL11" t="s">
         <v>41</v>
       </c>
-      <c r="AO11" s="2"/>
-    </row>
-    <row r="12" spans="1:41" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+      <c r="AP11" s="2"/>
+    </row>
+    <row r="12" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="Y12" s="12" t="s">
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="Z12" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="Z12" s="17" t="s">
+      <c r="AA12" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AA12" s="12" t="s">
+      <c r="AB12" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="AC12" s="15" t="s">
+      <c r="AD12" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AD12">
+      <c r="AE12">
         <v>0</v>
       </c>
-      <c r="AE12">
-        <v>1</v>
-      </c>
-      <c r="AJ12">
+      <c r="AF12">
+        <v>1</v>
+      </c>
+      <c r="AK12">
         <v>50</v>
       </c>
-      <c r="AK12" t="s">
+      <c r="AL12" t="s">
         <v>42</v>
       </c>
-      <c r="AL12" t="s">
+      <c r="AM12" t="s">
         <v>43</v>
       </c>
-      <c r="AO12" s="2"/>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
+      <c r="AP12" s="2"/>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="Y13" s="17" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="Z13" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="AA13" s="17" t="s">
+      <c r="AB13" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AC13" s="15" t="s">
+      <c r="AD13" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="AD13">
+      <c r="AE13">
         <v>0</v>
       </c>
-      <c r="AE13">
-        <v>1</v>
-      </c>
-      <c r="AJ13">
+      <c r="AF13">
+        <v>1</v>
+      </c>
+      <c r="AK13">
         <v>50</v>
       </c>
-      <c r="AK13" t="s">
+      <c r="AL13" t="s">
         <v>41</v>
       </c>
-      <c r="AO13" s="2"/>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="C14" s="10"/>
-      <c r="D14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="AO14" s="2"/>
-    </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="C15" s="7"/>
-      <c r="AO15" s="2"/>
-    </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="D16" s="7"/>
-      <c r="AO16" s="2"/>
-    </row>
-    <row r="17" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="D17" s="7"/>
-      <c r="AO17" s="2"/>
-    </row>
-    <row r="18" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="D18" s="7"/>
-      <c r="AO18" s="2"/>
-    </row>
-    <row r="19" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="D19" s="7"/>
-      <c r="AO19" s="2"/>
-    </row>
-    <row r="20" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="D20" s="7"/>
-      <c r="AO20" s="2"/>
-    </row>
-    <row r="21" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="D21" s="7"/>
-      <c r="AO21" s="2"/>
-    </row>
-    <row r="22" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C22" s="7"/>
-      <c r="AO22" s="2"/>
-    </row>
-    <row r="23" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C23" s="7"/>
-      <c r="AO23" s="2"/>
-    </row>
-    <row r="24" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C24" s="7"/>
-      <c r="AO24" s="2"/>
-    </row>
-    <row r="25" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C25" s="10"/>
-      <c r="D25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="AO25" s="2"/>
-    </row>
-    <row r="26" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C26" s="10"/>
-      <c r="D26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="AO26" s="2"/>
-    </row>
-    <row r="27" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C27" s="10"/>
-      <c r="D27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="AO27" s="2"/>
-    </row>
-    <row r="28" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C28" s="10"/>
-      <c r="D28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="AO28" s="2"/>
-    </row>
-    <row r="29" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="D29" s="10"/>
-      <c r="F29" s="9"/>
-      <c r="AO29" s="2"/>
-    </row>
-    <row r="30" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C30" s="10"/>
-      <c r="D30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="AO30" s="2"/>
-    </row>
-    <row r="31" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C31" s="7"/>
-      <c r="D31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="AO31" s="2"/>
-    </row>
-    <row r="32" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="D32" s="8"/>
-      <c r="F32" s="9"/>
-      <c r="AO32" s="2"/>
-    </row>
-    <row r="33" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="AO33" s="2"/>
-    </row>
-    <row r="34" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="AO34" s="2"/>
-    </row>
-    <row r="35" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C35" s="7"/>
-      <c r="AO35" s="2"/>
-    </row>
-    <row r="36" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C36" s="7"/>
-      <c r="AO36" s="2"/>
-    </row>
-    <row r="37" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="D37" s="8"/>
-      <c r="AO37" s="2"/>
-    </row>
-    <row r="38" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C38" s="7"/>
-      <c r="AO38" s="2"/>
-    </row>
-    <row r="39" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C39" s="7"/>
-      <c r="D39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="AO39" s="2"/>
-    </row>
-    <row r="40" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C40" s="7"/>
-      <c r="D40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="AO40" s="2"/>
-    </row>
-    <row r="41" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C41" s="7"/>
-      <c r="D41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="AO41" s="2"/>
-    </row>
-    <row r="42" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C42" s="7"/>
-      <c r="AO42" s="2"/>
-    </row>
-    <row r="43" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C43" s="7"/>
-      <c r="AO43" s="2"/>
-    </row>
-    <row r="44" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C44" s="7"/>
-      <c r="AO44" s="2"/>
-    </row>
-    <row r="45" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C45" s="7"/>
-      <c r="AO45" s="2"/>
-    </row>
-    <row r="46" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C46" s="7"/>
-      <c r="AO46" s="2"/>
-    </row>
-    <row r="47" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C47" s="7"/>
-      <c r="AO47" s="2"/>
-    </row>
-    <row r="48" spans="3:41" x14ac:dyDescent="0.2">
-      <c r="C48" s="7"/>
-      <c r="AO48" s="2"/>
-    </row>
-    <row r="49" spans="3:43" x14ac:dyDescent="0.2">
-      <c r="C49" s="7"/>
-      <c r="AO49" s="2"/>
-    </row>
-    <row r="50" spans="3:43" x14ac:dyDescent="0.2">
-      <c r="C50" s="7"/>
-      <c r="AO50" s="2"/>
-    </row>
-    <row r="51" spans="3:43" x14ac:dyDescent="0.2">
-      <c r="C51" s="7"/>
-      <c r="AO51" s="2"/>
-    </row>
-    <row r="52" spans="3:43" x14ac:dyDescent="0.2">
-      <c r="C52" s="7"/>
-      <c r="AO52" s="2"/>
-    </row>
-    <row r="53" spans="3:43" x14ac:dyDescent="0.2">
-      <c r="C53" s="7"/>
-      <c r="AO53" s="2"/>
-    </row>
-    <row r="54" spans="3:43" x14ac:dyDescent="0.2">
-      <c r="C54" s="8"/>
-      <c r="D54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="AO54" s="2"/>
-    </row>
-    <row r="55" spans="3:43" x14ac:dyDescent="0.2">
-      <c r="C55" s="8"/>
-      <c r="D55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="AO55" s="2"/>
-    </row>
-    <row r="56" spans="3:43" x14ac:dyDescent="0.2">
-      <c r="C56" s="10"/>
-      <c r="D56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="AO56" s="2"/>
-    </row>
-    <row r="57" spans="3:43" x14ac:dyDescent="0.2">
-      <c r="C57" s="7"/>
-      <c r="AO57" s="2"/>
-    </row>
-    <row r="58" spans="3:43" x14ac:dyDescent="0.2">
-      <c r="C58" s="7"/>
-      <c r="D58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="Y58" s="11"/>
-      <c r="AB58" s="11"/>
-      <c r="AO58" s="2"/>
-      <c r="AP58" s="1"/>
+      <c r="AP13" s="2"/>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A14" s="19"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="20"/>
+      <c r="X14" s="20"/>
+      <c r="Y14" s="20"/>
+      <c r="Z14" s="20"/>
+      <c r="AA14" s="20"/>
+      <c r="AB14" s="20"/>
+      <c r="AC14" s="20"/>
+      <c r="AD14" s="20"/>
+      <c r="AE14" s="20"/>
+      <c r="AF14" s="20"/>
+      <c r="AG14" s="20"/>
+      <c r="AH14" s="20"/>
+      <c r="AI14" s="20"/>
+      <c r="AJ14" s="20"/>
+      <c r="AK14" s="20"/>
+      <c r="AL14" s="20"/>
+      <c r="AM14" s="20"/>
+      <c r="AN14" s="20"/>
+      <c r="AO14" s="20"/>
+      <c r="AP14" s="20"/>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="D15" s="7"/>
+      <c r="AP15" s="2"/>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="E16" s="7"/>
+      <c r="AP16" s="2"/>
+    </row>
+    <row r="17" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="E17" s="7"/>
+      <c r="AP17" s="2"/>
+    </row>
+    <row r="18" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="E18" s="7"/>
+      <c r="AP18" s="2"/>
+    </row>
+    <row r="19" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="E19" s="7"/>
+      <c r="AP19" s="2"/>
+    </row>
+    <row r="20" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="E20" s="7"/>
+      <c r="AP20" s="2"/>
+    </row>
+    <row r="21" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="E21" s="7"/>
+      <c r="AP21" s="2"/>
+    </row>
+    <row r="22" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D22" s="7"/>
+      <c r="AP22" s="2"/>
+    </row>
+    <row r="23" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D23" s="7"/>
+      <c r="AP23" s="2"/>
+    </row>
+    <row r="24" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D24" s="7"/>
+      <c r="AP24" s="2"/>
+    </row>
+    <row r="25" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D25" s="10"/>
+      <c r="E25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="AP25" s="2"/>
+    </row>
+    <row r="26" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D26" s="10"/>
+      <c r="E26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="AP26" s="2"/>
+    </row>
+    <row r="27" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D27" s="10"/>
+      <c r="E27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="AP27" s="2"/>
+    </row>
+    <row r="28" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D28" s="10"/>
+      <c r="E28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="AP28" s="2"/>
+    </row>
+    <row r="29" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="E29" s="10"/>
+      <c r="G29" s="9"/>
+      <c r="AP29" s="2"/>
+    </row>
+    <row r="30" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D30" s="10"/>
+      <c r="E30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="AP30" s="2"/>
+    </row>
+    <row r="31" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D31" s="7"/>
+      <c r="E31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="AP31" s="2"/>
+    </row>
+    <row r="32" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="E32" s="8"/>
+      <c r="G32" s="9"/>
+      <c r="AP32" s="2"/>
+    </row>
+    <row r="33" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D33" s="8"/>
+      <c r="E33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="AP33" s="2"/>
+    </row>
+    <row r="34" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D34" s="8"/>
+      <c r="E34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="AP34" s="2"/>
+    </row>
+    <row r="35" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D35" s="7"/>
+      <c r="AP35" s="2"/>
+    </row>
+    <row r="36" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D36" s="7"/>
+      <c r="AP36" s="2"/>
+    </row>
+    <row r="37" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="E37" s="8"/>
+      <c r="AP37" s="2"/>
+    </row>
+    <row r="38" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D38" s="7"/>
+      <c r="AP38" s="2"/>
+    </row>
+    <row r="39" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D39" s="7"/>
+      <c r="E39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="AP39" s="2"/>
+    </row>
+    <row r="40" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D40" s="7"/>
+      <c r="E40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="AP40" s="2"/>
+    </row>
+    <row r="41" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D41" s="7"/>
+      <c r="E41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="AP41" s="2"/>
+    </row>
+    <row r="42" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D42" s="7"/>
+      <c r="AP42" s="2"/>
+    </row>
+    <row r="43" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D43" s="7"/>
+      <c r="AP43" s="2"/>
+    </row>
+    <row r="44" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D44" s="7"/>
+      <c r="AP44" s="2"/>
+    </row>
+    <row r="45" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D45" s="7"/>
+      <c r="AP45" s="2"/>
+    </row>
+    <row r="46" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D46" s="7"/>
+      <c r="AP46" s="2"/>
+    </row>
+    <row r="47" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D47" s="7"/>
+      <c r="AP47" s="2"/>
+    </row>
+    <row r="48" spans="4:42" x14ac:dyDescent="0.2">
+      <c r="D48" s="7"/>
+      <c r="AP48" s="2"/>
+    </row>
+    <row r="49" spans="4:44" x14ac:dyDescent="0.2">
+      <c r="D49" s="7"/>
+      <c r="AP49" s="2"/>
+    </row>
+    <row r="50" spans="4:44" x14ac:dyDescent="0.2">
+      <c r="D50" s="7"/>
+      <c r="AP50" s="2"/>
+    </row>
+    <row r="51" spans="4:44" x14ac:dyDescent="0.2">
+      <c r="D51" s="7"/>
+      <c r="AP51" s="2"/>
+    </row>
+    <row r="52" spans="4:44" x14ac:dyDescent="0.2">
+      <c r="D52" s="7"/>
+      <c r="AP52" s="2"/>
+    </row>
+    <row r="53" spans="4:44" x14ac:dyDescent="0.2">
+      <c r="D53" s="7"/>
+      <c r="AP53" s="2"/>
+    </row>
+    <row r="54" spans="4:44" x14ac:dyDescent="0.2">
+      <c r="D54" s="8"/>
+      <c r="E54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="AP54" s="2"/>
+    </row>
+    <row r="55" spans="4:44" x14ac:dyDescent="0.2">
+      <c r="D55" s="8"/>
+      <c r="E55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="AP55" s="2"/>
+    </row>
+    <row r="56" spans="4:44" x14ac:dyDescent="0.2">
+      <c r="D56" s="10"/>
+      <c r="E56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="AP56" s="2"/>
+    </row>
+    <row r="57" spans="4:44" x14ac:dyDescent="0.2">
+      <c r="D57" s="7"/>
+      <c r="AP57" s="2"/>
+    </row>
+    <row r="58" spans="4:44" x14ac:dyDescent="0.2">
+      <c r="D58" s="7"/>
+      <c r="E58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="Z58" s="11"/>
+      <c r="AC58" s="11"/>
+      <c r="AP58" s="2"/>
       <c r="AQ58" s="1"/>
-    </row>
-    <row r="59" spans="3:43" x14ac:dyDescent="0.2">
-      <c r="C59" s="7"/>
-      <c r="D59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="AN59" s="1"/>
-      <c r="AO59" s="2"/>
-      <c r="AP59" s="1"/>
+      <c r="AR58" s="1"/>
+    </row>
+    <row r="59" spans="4:44" x14ac:dyDescent="0.2">
+      <c r="D59" s="7"/>
+      <c r="E59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="AO59" s="1"/>
+      <c r="AP59" s="2"/>
       <c r="AQ59" s="1"/>
-    </row>
-    <row r="60" spans="3:43" x14ac:dyDescent="0.2">
-      <c r="C60" s="7"/>
-      <c r="D60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="AN60" s="1"/>
-      <c r="AO60" s="2"/>
-    </row>
-    <row r="61" spans="3:43" x14ac:dyDescent="0.2">
-      <c r="C61" s="7"/>
-      <c r="AO61" s="2"/>
-    </row>
-    <row r="62" spans="3:43" x14ac:dyDescent="0.2">
-      <c r="C62" s="7"/>
-      <c r="AO62" s="2"/>
-    </row>
-    <row r="63" spans="3:43" x14ac:dyDescent="0.2">
-      <c r="C63" s="7"/>
-      <c r="D63" s="9"/>
+      <c r="AR59" s="1"/>
+    </row>
+    <row r="60" spans="4:44" x14ac:dyDescent="0.2">
+      <c r="D60" s="7"/>
+      <c r="E60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="AO60" s="1"/>
+      <c r="AP60" s="2"/>
+    </row>
+    <row r="61" spans="4:44" x14ac:dyDescent="0.2">
+      <c r="D61" s="7"/>
+      <c r="AP61" s="2"/>
+    </row>
+    <row r="62" spans="4:44" x14ac:dyDescent="0.2">
+      <c r="D62" s="7"/>
+      <c r="AP62" s="2"/>
+    </row>
+    <row r="63" spans="4:44" x14ac:dyDescent="0.2">
+      <c r="D63" s="7"/>
+      <c r="E63" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO62" xr:uid="{C991D8A7-FC2B-1B42-8758-01766B2FD0CA}"/>
+  <autoFilter ref="B1:AP62" xr:uid="{C991D8A7-FC2B-1B42-8758-01766B2FD0CA}"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>